<commit_message>
Agregando Login, CalculadoraIMC, ContadorDS(Pendiente)
</commit_message>
<xml_diff>
--- a/capitalized_text.xlsx
+++ b/capitalized_text.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,13 +431,6 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Camila</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
           <t>Gonzalo</t>
         </is>
       </c>

</xml_diff>